<commit_message>
Updated project For Admin Side
</commit_message>
<xml_diff>
--- a/sample_data/28 JUNE 2023 CFS.xlsx
+++ b/sample_data/28 JUNE 2023 CFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6790"/>
+    <workbookView windowWidth="18350" windowHeight="6830"/>
   </bookViews>
   <sheets>
     <sheet name="export - 2023-06-28T100116.389" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1090,7 +1090,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>

</xml_diff>